<commit_message>
MVsB5_BT_Audio_SDK_V0.5.0 - *.pdf *.doc *.xlsx
</commit_message>
<xml_diff>
--- a/BT_Audio_APP/middleware/roboeffect/third_party_effect/simple_gain/UserLibsData.xlsx
+++ b/BT_Audio_APP/middleware/roboeffect/third_party_effect/simple_gain/UserLibsData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\castle_work\du360\DU56x\v3_engine_codes\codes\roboeffect_svn_20230427\middleware\roboeffect\3rd_part_effect\simple_gain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\castle_work\du360\DU56x\v3_engine_codes\codes\roboeffect_svn_20230427\middleware\roboeffect\third_party_effect\simple_gain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C485564-7B9A-4894-8AE6-17D721F306B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFE1835-DE22-478D-8D1B-D9E6CA2CFCB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30000" windowHeight="17496" tabRatio="867" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,8 +19,408 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>蔡晓俊</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{0AE33EF5-5CB7-48CA-A62F-222AB5B24A17}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Castle:
+填入自定义音效名称，遵循C语言变量的规范，注意：需和sheet名称，外围目录名称保持一致</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{75051EFD-7EC6-4FA6-921C-13FA5CD69064}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Castle:
+数据位宽支持，请遵下拉列表提供的值进行填写</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{4C56FDE0-E0B3-4E9A-96C2-589F3ACD333C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Castle:
+第一输入源声道数支持，请遵下拉列表提供的值进行填写</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{D04185CF-DCCF-45B0-8471-7C53D3D06AF2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Castle:
+第二输入源声道数支持，请遵下拉列表提供的值进行填写</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{7B5E2078-52E4-4446-9485-4796405FEA11}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Castle:
+输出声道数支持，请遵下拉列表提供的值进行填写</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{1B3C9BD2-7C6E-4766-B937-00923551C3F9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Castle:
+缺省false，不用修改</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{5EF5FE2E-1A64-433C-A10F-675EBF9465D1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>支持的帧长数：
+A.如果是任意长度，填FZ_ANY
+B.也可以填FZ_64,FZ_128,FZ_256,FZ_512，甚至是这些值的任意组合，用或运算符连接，如FZ_128|FZ_256。
+C.如果是一个特殊帧长，如320，请填写FZ_ANY,然后在roboeffect_xxxxx_memory_size_if接口内校验传入的参数if(query-&gt;frame_size == 320) 做动态判断。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{37169ECC-1813-40D9-BBF7-8610840AB326}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Castle:
+参数UI空间的布局
+一般情况alyout填auto即可</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{FB77282B-446C-4F34-B952-AED2113A1F9A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Castle:
+参数名称，按C语言变量风格填写</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{BCE1BD74-B219-4795-9BB4-CBB22CD192E4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Castle:
+参数类型选择，请按下拉列表提供的值选择。
+bool 布尔型，只提供0或者1的值
+enum 枚举型，按照context提供的序列，从0到N排列获得值
+value 数值型，按照context提供的范围和步进获得值
+display 显示型，用于返回计算结果，比如通过音效算法获得信号幅度，噪声等级，等等。</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{15095CCB-67AC-48D4-A889-3CE275DD5EE9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Castle:
+参数内容，如何填写和参数类型相关：
+bool布尔型：不用填写
+enum枚举型：按不同的枚举文本字串以分号连接，如: one;two;three;four，调音工具以此显示这些字串的下拉列表，设置参数时，"one"的值为0，"two"的值为1，"three"的值为2，以此类推。
+value数值型：需要按 XXXX,YYYY,ZZZZ填写，其中：
+XXXX 代表这个参数的下限
+YYYY 代表这个参数的上限
+ZZZZ 代表调节参数时的步进
+display显示型：需要按 XXXX,YYYY填写，其中：
+XXXX 代表这个参数的下限
+YYYY 代表这个参数的上限</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{2491968D-5536-4C74-B509-EFE963B0B937}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Castle:
+参数的缺省值
+如果是enum枚举型，请填写实际的参数值，
+如 "one;two;three;four" 需要将three作为缺省值，请填2</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{F5191FBB-00ED-4D22-B5AC-34F6B8306FFE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Castle:
+参数配置，主要描述了</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <u/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>当参数变化</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>时，需要调用的api接口，
+请按照下拉列表提供的值填写，每个值代表的含义如下：
+METHOD_NONE: 不需要调用任何方法进行配置，改变后的参数直接传入apply接口即可生效。
+METHOD_INIT: 此参数变化后，需要重新调用init接口对音效进行初始化。
+METHOD_CFG_1: 此参数变化后，需要调用特定的音效配置函数，
+请关注roboeffect_xxxx_config_if接口中的特定代码进行调用：
+if((method_flag &amp; METHOD_CFG_1) &amp;&amp; info.is_active)
+{
+  //Todo: call APIs to config parameters
+}
+METHOD_CFG_2 和 METHOD_CFG_3 同 METHOD_CFG_1，做一个分类而已：
+if((method_flag &amp; METHOD_CFG_2) &amp;&amp; info.is_active)
+{
+  //Todo: call APIs to config parameters
+}
+METHOD_CFG_FADEOI
+METHOD_CFG_STEP
+系统保留，目前不使用</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{811A40D0-6E07-4A1F-BF62-53C56E508D31}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Castle:
+此参数在上位机工具中的UI显示类型，需要和参数类型对应相关
+bool布尔型可以使用的类型：check_box, push_button
+enum枚举型可以使用的类型：comb_box
+value数值型可以使用的类型：spinbox, hslider, vsilder, dial
+display显示型可以使用的类型：label, progress_bar, on_off
+请不要对应错误，以免出现显示问题。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{401BF186-94A2-4856-BF00-A79F8EE2AE79}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Castle:
+参数单位，可以不填
+只有数值型和显示型可以使用。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{16FAAF56-A81F-4B2E-908D-FA1365B27452}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Castle:
+参数保留的小数
+只有数值型和显示型可以使用。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K4" authorId="0" shapeId="0" xr:uid="{61E4700A-171D-416B-9BBA-D4A0B0DB2854}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Castle:
+参数真实传输的数值,和显示的数值的比率
+由于调音协议中只定义了int16整形，如果要显示小数，需要约定保留的小数位数和转换方式。
+比如：参数值为1234，调音显示值为12.34，真实传输的值为1234，那么fract=2, ratio=100，保证音效api收到的值为1234
+也存在某些情况，比如需要使用Q6.10格式传输，那么ratio=1024，显示值0.25，传输值为0.25*1024=256
+只有数值型和显示型可以使用。</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L4" authorId="0" shapeId="0" xr:uid="{C4C43E52-123E-4A9B-9A27-5AF6014606E6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Castle:
+参数提示，类似comment，可以填入文本，上位机调音时，鼠标放到参数上可以显示这段文本。</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t>version</t>
   </si>
@@ -56,9 +456,6 @@
   </si>
   <si>
     <t>fz</t>
-  </si>
-  <si>
-    <t>cnx_name</t>
   </si>
   <si>
     <t>false</t>
@@ -178,17 +575,13 @@
   </si>
   <si>
     <t>simple_gain</t>
-  </si>
-  <si>
-    <t>(sizeof(simple_gain_struct))</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -210,6 +603,30 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="6">
@@ -423,7 +840,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -827,16 +1244,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.21875" style="13" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5546875" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.88671875" style="13" customWidth="1"/>
@@ -850,8 +1267,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>51</v>
+      <c r="A1" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -874,17 +1291,15 @@
       <c r="H1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="I1" s="7"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="9"/>
       <c r="M1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" s="13" t="s">
         <v>46</v>
-      </c>
-      <c r="S1" s="13" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -905,30 +1320,28 @@
         <v>2</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I2" t="s">
-        <v>52</v>
-      </c>
+      <c r="I2" s="15"/>
       <c r="J2" s="2"/>
       <c r="K2" s="5"/>
       <c r="L2" s="3"/>
       <c r="Q2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" s="11" t="s">
         <v>14</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>17</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
@@ -936,7 +1349,7 @@
       <c r="F3" s="17"/>
       <c r="G3" s="18"/>
       <c r="H3" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
@@ -944,114 +1357,114 @@
       <c r="L3" s="20"/>
       <c r="M3" s="21"/>
       <c r="N3" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O3" s="20"/>
       <c r="P3" s="21"/>
       <c r="Q3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" s="13" t="s">
         <v>20</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="F5" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>42</v>
-      </c>
       <c r="N5" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O5" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="I6" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="N6" s="13" t="s">
-        <v>38</v>
-      </c>
       <c r="O6" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1082,11 +1495,8 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{00000000-0002-0000-3B00-000006000000}">
       <formula1>"false,true"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H5:H27" xr:uid="{00000000-0002-0000-3B00-000007000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H7:H27" xr:uid="{00000000-0002-0000-3B00-000007000000}">
       <formula1>"check_box,push_button,comb_box,spinbox,hslider,vsilder,label,progress_bar,on_off"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H5:H6" xr:uid="{00000000-0002-0000-3B00-000008000000}">
-      <formula1>"check_box,push_button,comb_box,spinbox,hslider,vsilder,label,progress_bar"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A3" xr:uid="{00000000-0002-0000-3B00-000009000000}">
       <formula1>"scratch,no scratch"</formula1>
@@ -1097,8 +1507,12 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C5:C56" xr:uid="{00000000-0002-0000-3B00-000001000000}">
       <formula1>"bool,enum,value,display"</formula1>
     </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H5:H6" xr:uid="{CBF30F6A-8363-4451-9330-EFA8091D6B81}">
+      <formula1>"check_box,push_button,on_off,comb_box,spinbox,hslider,vsilder,dial,label,progress_bar,"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>